<commit_message>
[DROOLS-1564] change oopath syntax
</commit_message>
<xml_diff>
--- a/drools-test-coverage/test-suite/src/test/resources/org/drools/testcoverage/functional/oopath/oopath.xlsx
+++ b/drools-test-coverage/test-suite/src/test/resources/org/drools/testcoverage/functional/oopath/oopath.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" state="visible" r:id="rId2"/>
@@ -46,7 +46,7 @@
   </si>
   <si>
     <t xml:space="preserve">query listSafeCities
-$cities : List() from accumulate (Person ( $city: /address{#InternationalAddress, state == "Safecountry"}/city), collectList($city))
+$cities : List() from accumulate (Person ( $city: /address#InternationalAddress[state == "Safecountry"]/city), collectList($city))
 end</t>
   </si>
   <si>
@@ -65,7 +65,7 @@
     <t xml:space="preserve">list</t>
   </si>
   <si>
-    <t xml:space="preserve">/address{#InternationalAddress, state  == "$param"}</t>
+    <t xml:space="preserve">/address#InternationalAddress[state  == "$param"]</t>
   </si>
   <si>
     <t xml:space="preserve">age &gt; $param</t>
@@ -141,6 +141,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -161,6 +162,7 @@
       <sz val="7"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -168,6 +170,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -175,18 +178,21 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="7"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -317,9 +323,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -388,10 +396,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -421,10 +425,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -450,26 +450,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IU15"/>
+  <dimension ref="A1:IW15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="45.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="51.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="20.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="257" min="11" style="1" width="9.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="258" style="0" width="9.08"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="44.6836734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.75"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="51.2959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="257" min="11" style="1" width="9.04591836734694"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -479,7 +478,7 @@
       <c r="D1" s="3"/>
       <c r="IU1" s="0"/>
     </row>
-    <row r="2" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -488,12 +487,261 @@
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
+      <c r="E2" s="0"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
+      <c r="M2" s="0"/>
+      <c r="N2" s="0"/>
+      <c r="O2" s="0"/>
+      <c r="P2" s="0"/>
+      <c r="Q2" s="0"/>
+      <c r="R2" s="0"/>
+      <c r="S2" s="0"/>
+      <c r="T2" s="0"/>
+      <c r="U2" s="0"/>
+      <c r="V2" s="0"/>
+      <c r="W2" s="0"/>
+      <c r="X2" s="0"/>
+      <c r="Y2" s="0"/>
+      <c r="Z2" s="0"/>
+      <c r="AA2" s="0"/>
+      <c r="AB2" s="0"/>
+      <c r="AC2" s="0"/>
+      <c r="AD2" s="0"/>
+      <c r="AE2" s="0"/>
+      <c r="AF2" s="0"/>
+      <c r="AG2" s="0"/>
+      <c r="AH2" s="0"/>
+      <c r="AI2" s="0"/>
+      <c r="AJ2" s="0"/>
+      <c r="AK2" s="0"/>
+      <c r="AL2" s="0"/>
+      <c r="AM2" s="0"/>
+      <c r="AN2" s="0"/>
+      <c r="AO2" s="0"/>
+      <c r="AP2" s="0"/>
+      <c r="AQ2" s="0"/>
+      <c r="AR2" s="0"/>
+      <c r="AS2" s="0"/>
+      <c r="AT2" s="0"/>
+      <c r="AU2" s="0"/>
+      <c r="AV2" s="0"/>
+      <c r="AW2" s="0"/>
+      <c r="AX2" s="0"/>
+      <c r="AY2" s="0"/>
+      <c r="AZ2" s="0"/>
+      <c r="BA2" s="0"/>
+      <c r="BB2" s="0"/>
+      <c r="BC2" s="0"/>
+      <c r="BD2" s="0"/>
+      <c r="BE2" s="0"/>
+      <c r="BF2" s="0"/>
+      <c r="BG2" s="0"/>
+      <c r="BH2" s="0"/>
+      <c r="BI2" s="0"/>
+      <c r="BJ2" s="0"/>
+      <c r="BK2" s="0"/>
+      <c r="BL2" s="0"/>
+      <c r="BM2" s="0"/>
+      <c r="BN2" s="0"/>
+      <c r="BO2" s="0"/>
+      <c r="BP2" s="0"/>
+      <c r="BQ2" s="0"/>
+      <c r="BR2" s="0"/>
+      <c r="BS2" s="0"/>
+      <c r="BT2" s="0"/>
+      <c r="BU2" s="0"/>
+      <c r="BV2" s="0"/>
+      <c r="BW2" s="0"/>
+      <c r="BX2" s="0"/>
+      <c r="BY2" s="0"/>
+      <c r="BZ2" s="0"/>
+      <c r="CA2" s="0"/>
+      <c r="CB2" s="0"/>
+      <c r="CC2" s="0"/>
+      <c r="CD2" s="0"/>
+      <c r="CE2" s="0"/>
+      <c r="CF2" s="0"/>
+      <c r="CG2" s="0"/>
+      <c r="CH2" s="0"/>
+      <c r="CI2" s="0"/>
+      <c r="CJ2" s="0"/>
+      <c r="CK2" s="0"/>
+      <c r="CL2" s="0"/>
+      <c r="CM2" s="0"/>
+      <c r="CN2" s="0"/>
+      <c r="CO2" s="0"/>
+      <c r="CP2" s="0"/>
+      <c r="CQ2" s="0"/>
+      <c r="CR2" s="0"/>
+      <c r="CS2" s="0"/>
+      <c r="CT2" s="0"/>
+      <c r="CU2" s="0"/>
+      <c r="CV2" s="0"/>
+      <c r="CW2" s="0"/>
+      <c r="CX2" s="0"/>
+      <c r="CY2" s="0"/>
+      <c r="CZ2" s="0"/>
+      <c r="DA2" s="0"/>
+      <c r="DB2" s="0"/>
+      <c r="DC2" s="0"/>
+      <c r="DD2" s="0"/>
+      <c r="DE2" s="0"/>
+      <c r="DF2" s="0"/>
+      <c r="DG2" s="0"/>
+      <c r="DH2" s="0"/>
+      <c r="DI2" s="0"/>
+      <c r="DJ2" s="0"/>
+      <c r="DK2" s="0"/>
+      <c r="DL2" s="0"/>
+      <c r="DM2" s="0"/>
+      <c r="DN2" s="0"/>
+      <c r="DO2" s="0"/>
+      <c r="DP2" s="0"/>
+      <c r="DQ2" s="0"/>
+      <c r="DR2" s="0"/>
+      <c r="DS2" s="0"/>
+      <c r="DT2" s="0"/>
+      <c r="DU2" s="0"/>
+      <c r="DV2" s="0"/>
+      <c r="DW2" s="0"/>
+      <c r="DX2" s="0"/>
+      <c r="DY2" s="0"/>
+      <c r="DZ2" s="0"/>
+      <c r="EA2" s="0"/>
+      <c r="EB2" s="0"/>
+      <c r="EC2" s="0"/>
+      <c r="ED2" s="0"/>
+      <c r="EE2" s="0"/>
+      <c r="EF2" s="0"/>
+      <c r="EG2" s="0"/>
+      <c r="EH2" s="0"/>
+      <c r="EI2" s="0"/>
+      <c r="EJ2" s="0"/>
+      <c r="EK2" s="0"/>
+      <c r="EL2" s="0"/>
+      <c r="EM2" s="0"/>
+      <c r="EN2" s="0"/>
+      <c r="EO2" s="0"/>
+      <c r="EP2" s="0"/>
+      <c r="EQ2" s="0"/>
+      <c r="ER2" s="0"/>
+      <c r="ES2" s="0"/>
+      <c r="ET2" s="0"/>
+      <c r="EU2" s="0"/>
+      <c r="EV2" s="0"/>
+      <c r="EW2" s="0"/>
+      <c r="EX2" s="0"/>
+      <c r="EY2" s="0"/>
+      <c r="EZ2" s="0"/>
+      <c r="FA2" s="0"/>
+      <c r="FB2" s="0"/>
+      <c r="FC2" s="0"/>
+      <c r="FD2" s="0"/>
+      <c r="FE2" s="0"/>
+      <c r="FF2" s="0"/>
+      <c r="FG2" s="0"/>
+      <c r="FH2" s="0"/>
+      <c r="FI2" s="0"/>
+      <c r="FJ2" s="0"/>
+      <c r="FK2" s="0"/>
+      <c r="FL2" s="0"/>
+      <c r="FM2" s="0"/>
+      <c r="FN2" s="0"/>
+      <c r="FO2" s="0"/>
+      <c r="FP2" s="0"/>
+      <c r="FQ2" s="0"/>
+      <c r="FR2" s="0"/>
+      <c r="FS2" s="0"/>
+      <c r="FT2" s="0"/>
+      <c r="FU2" s="0"/>
+      <c r="FV2" s="0"/>
+      <c r="FW2" s="0"/>
+      <c r="FX2" s="0"/>
+      <c r="FY2" s="0"/>
+      <c r="FZ2" s="0"/>
+      <c r="GA2" s="0"/>
+      <c r="GB2" s="0"/>
+      <c r="GC2" s="0"/>
+      <c r="GD2" s="0"/>
+      <c r="GE2" s="0"/>
+      <c r="GF2" s="0"/>
+      <c r="GG2" s="0"/>
+      <c r="GH2" s="0"/>
+      <c r="GI2" s="0"/>
+      <c r="GJ2" s="0"/>
+      <c r="GK2" s="0"/>
+      <c r="GL2" s="0"/>
+      <c r="GM2" s="0"/>
+      <c r="GN2" s="0"/>
+      <c r="GO2" s="0"/>
+      <c r="GP2" s="0"/>
+      <c r="GQ2" s="0"/>
+      <c r="GR2" s="0"/>
+      <c r="GS2" s="0"/>
+      <c r="GT2" s="0"/>
+      <c r="GU2" s="0"/>
+      <c r="GV2" s="0"/>
+      <c r="GW2" s="0"/>
+      <c r="GX2" s="0"/>
+      <c r="GY2" s="0"/>
+      <c r="GZ2" s="0"/>
+      <c r="HA2" s="0"/>
+      <c r="HB2" s="0"/>
+      <c r="HC2" s="0"/>
+      <c r="HD2" s="0"/>
+      <c r="HE2" s="0"/>
+      <c r="HF2" s="0"/>
+      <c r="HG2" s="0"/>
+      <c r="HH2" s="0"/>
+      <c r="HI2" s="0"/>
+      <c r="HJ2" s="0"/>
+      <c r="HK2" s="0"/>
+      <c r="HL2" s="0"/>
+      <c r="HM2" s="0"/>
+      <c r="HN2" s="0"/>
+      <c r="HO2" s="0"/>
+      <c r="HP2" s="0"/>
+      <c r="HQ2" s="0"/>
+      <c r="HR2" s="0"/>
+      <c r="HS2" s="0"/>
+      <c r="HT2" s="0"/>
+      <c r="HU2" s="0"/>
+      <c r="HV2" s="0"/>
+      <c r="HW2" s="0"/>
+      <c r="HX2" s="0"/>
+      <c r="HY2" s="0"/>
+      <c r="HZ2" s="0"/>
+      <c r="IA2" s="0"/>
+      <c r="IB2" s="0"/>
+      <c r="IC2" s="0"/>
+      <c r="ID2" s="0"/>
+      <c r="IE2" s="0"/>
+      <c r="IF2" s="0"/>
+      <c r="IG2" s="0"/>
+      <c r="IH2" s="0"/>
+      <c r="II2" s="0"/>
+      <c r="IJ2" s="0"/>
+      <c r="IK2" s="0"/>
+      <c r="IL2" s="0"/>
+      <c r="IM2" s="0"/>
+      <c r="IN2" s="0"/>
+      <c r="IO2" s="0"/>
+      <c r="IP2" s="0"/>
+      <c r="IQ2" s="0"/>
+      <c r="IR2" s="0"/>
+      <c r="IS2" s="0"/>
+      <c r="IT2" s="0"/>
       <c r="IU2" s="0"/>
+      <c r="IV2" s="0"/>
+      <c r="IW2" s="0"/>
     </row>
-    <row r="3" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -502,10 +750,259 @@
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
+      <c r="E3" s="0"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
+      <c r="L3" s="0"/>
+      <c r="M3" s="0"/>
+      <c r="N3" s="0"/>
+      <c r="O3" s="0"/>
+      <c r="P3" s="0"/>
+      <c r="Q3" s="0"/>
+      <c r="R3" s="0"/>
+      <c r="S3" s="0"/>
+      <c r="T3" s="0"/>
+      <c r="U3" s="0"/>
+      <c r="V3" s="0"/>
+      <c r="W3" s="0"/>
+      <c r="X3" s="0"/>
+      <c r="Y3" s="0"/>
+      <c r="Z3" s="0"/>
+      <c r="AA3" s="0"/>
+      <c r="AB3" s="0"/>
+      <c r="AC3" s="0"/>
+      <c r="AD3" s="0"/>
+      <c r="AE3" s="0"/>
+      <c r="AF3" s="0"/>
+      <c r="AG3" s="0"/>
+      <c r="AH3" s="0"/>
+      <c r="AI3" s="0"/>
+      <c r="AJ3" s="0"/>
+      <c r="AK3" s="0"/>
+      <c r="AL3" s="0"/>
+      <c r="AM3" s="0"/>
+      <c r="AN3" s="0"/>
+      <c r="AO3" s="0"/>
+      <c r="AP3" s="0"/>
+      <c r="AQ3" s="0"/>
+      <c r="AR3" s="0"/>
+      <c r="AS3" s="0"/>
+      <c r="AT3" s="0"/>
+      <c r="AU3" s="0"/>
+      <c r="AV3" s="0"/>
+      <c r="AW3" s="0"/>
+      <c r="AX3" s="0"/>
+      <c r="AY3" s="0"/>
+      <c r="AZ3" s="0"/>
+      <c r="BA3" s="0"/>
+      <c r="BB3" s="0"/>
+      <c r="BC3" s="0"/>
+      <c r="BD3" s="0"/>
+      <c r="BE3" s="0"/>
+      <c r="BF3" s="0"/>
+      <c r="BG3" s="0"/>
+      <c r="BH3" s="0"/>
+      <c r="BI3" s="0"/>
+      <c r="BJ3" s="0"/>
+      <c r="BK3" s="0"/>
+      <c r="BL3" s="0"/>
+      <c r="BM3" s="0"/>
+      <c r="BN3" s="0"/>
+      <c r="BO3" s="0"/>
+      <c r="BP3" s="0"/>
+      <c r="BQ3" s="0"/>
+      <c r="BR3" s="0"/>
+      <c r="BS3" s="0"/>
+      <c r="BT3" s="0"/>
+      <c r="BU3" s="0"/>
+      <c r="BV3" s="0"/>
+      <c r="BW3" s="0"/>
+      <c r="BX3" s="0"/>
+      <c r="BY3" s="0"/>
+      <c r="BZ3" s="0"/>
+      <c r="CA3" s="0"/>
+      <c r="CB3" s="0"/>
+      <c r="CC3" s="0"/>
+      <c r="CD3" s="0"/>
+      <c r="CE3" s="0"/>
+      <c r="CF3" s="0"/>
+      <c r="CG3" s="0"/>
+      <c r="CH3" s="0"/>
+      <c r="CI3" s="0"/>
+      <c r="CJ3" s="0"/>
+      <c r="CK3" s="0"/>
+      <c r="CL3" s="0"/>
+      <c r="CM3" s="0"/>
+      <c r="CN3" s="0"/>
+      <c r="CO3" s="0"/>
+      <c r="CP3" s="0"/>
+      <c r="CQ3" s="0"/>
+      <c r="CR3" s="0"/>
+      <c r="CS3" s="0"/>
+      <c r="CT3" s="0"/>
+      <c r="CU3" s="0"/>
+      <c r="CV3" s="0"/>
+      <c r="CW3" s="0"/>
+      <c r="CX3" s="0"/>
+      <c r="CY3" s="0"/>
+      <c r="CZ3" s="0"/>
+      <c r="DA3" s="0"/>
+      <c r="DB3" s="0"/>
+      <c r="DC3" s="0"/>
+      <c r="DD3" s="0"/>
+      <c r="DE3" s="0"/>
+      <c r="DF3" s="0"/>
+      <c r="DG3" s="0"/>
+      <c r="DH3" s="0"/>
+      <c r="DI3" s="0"/>
+      <c r="DJ3" s="0"/>
+      <c r="DK3" s="0"/>
+      <c r="DL3" s="0"/>
+      <c r="DM3" s="0"/>
+      <c r="DN3" s="0"/>
+      <c r="DO3" s="0"/>
+      <c r="DP3" s="0"/>
+      <c r="DQ3" s="0"/>
+      <c r="DR3" s="0"/>
+      <c r="DS3" s="0"/>
+      <c r="DT3" s="0"/>
+      <c r="DU3" s="0"/>
+      <c r="DV3" s="0"/>
+      <c r="DW3" s="0"/>
+      <c r="DX3" s="0"/>
+      <c r="DY3" s="0"/>
+      <c r="DZ3" s="0"/>
+      <c r="EA3" s="0"/>
+      <c r="EB3" s="0"/>
+      <c r="EC3" s="0"/>
+      <c r="ED3" s="0"/>
+      <c r="EE3" s="0"/>
+      <c r="EF3" s="0"/>
+      <c r="EG3" s="0"/>
+      <c r="EH3" s="0"/>
+      <c r="EI3" s="0"/>
+      <c r="EJ3" s="0"/>
+      <c r="EK3" s="0"/>
+      <c r="EL3" s="0"/>
+      <c r="EM3" s="0"/>
+      <c r="EN3" s="0"/>
+      <c r="EO3" s="0"/>
+      <c r="EP3" s="0"/>
+      <c r="EQ3" s="0"/>
+      <c r="ER3" s="0"/>
+      <c r="ES3" s="0"/>
+      <c r="ET3" s="0"/>
+      <c r="EU3" s="0"/>
+      <c r="EV3" s="0"/>
+      <c r="EW3" s="0"/>
+      <c r="EX3" s="0"/>
+      <c r="EY3" s="0"/>
+      <c r="EZ3" s="0"/>
+      <c r="FA3" s="0"/>
+      <c r="FB3" s="0"/>
+      <c r="FC3" s="0"/>
+      <c r="FD3" s="0"/>
+      <c r="FE3" s="0"/>
+      <c r="FF3" s="0"/>
+      <c r="FG3" s="0"/>
+      <c r="FH3" s="0"/>
+      <c r="FI3" s="0"/>
+      <c r="FJ3" s="0"/>
+      <c r="FK3" s="0"/>
+      <c r="FL3" s="0"/>
+      <c r="FM3" s="0"/>
+      <c r="FN3" s="0"/>
+      <c r="FO3" s="0"/>
+      <c r="FP3" s="0"/>
+      <c r="FQ3" s="0"/>
+      <c r="FR3" s="0"/>
+      <c r="FS3" s="0"/>
+      <c r="FT3" s="0"/>
+      <c r="FU3" s="0"/>
+      <c r="FV3" s="0"/>
+      <c r="FW3" s="0"/>
+      <c r="FX3" s="0"/>
+      <c r="FY3" s="0"/>
+      <c r="FZ3" s="0"/>
+      <c r="GA3" s="0"/>
+      <c r="GB3" s="0"/>
+      <c r="GC3" s="0"/>
+      <c r="GD3" s="0"/>
+      <c r="GE3" s="0"/>
+      <c r="GF3" s="0"/>
+      <c r="GG3" s="0"/>
+      <c r="GH3" s="0"/>
+      <c r="GI3" s="0"/>
+      <c r="GJ3" s="0"/>
+      <c r="GK3" s="0"/>
+      <c r="GL3" s="0"/>
+      <c r="GM3" s="0"/>
+      <c r="GN3" s="0"/>
+      <c r="GO3" s="0"/>
+      <c r="GP3" s="0"/>
+      <c r="GQ3" s="0"/>
+      <c r="GR3" s="0"/>
+      <c r="GS3" s="0"/>
+      <c r="GT3" s="0"/>
+      <c r="GU3" s="0"/>
+      <c r="GV3" s="0"/>
+      <c r="GW3" s="0"/>
+      <c r="GX3" s="0"/>
+      <c r="GY3" s="0"/>
+      <c r="GZ3" s="0"/>
+      <c r="HA3" s="0"/>
+      <c r="HB3" s="0"/>
+      <c r="HC3" s="0"/>
+      <c r="HD3" s="0"/>
+      <c r="HE3" s="0"/>
+      <c r="HF3" s="0"/>
+      <c r="HG3" s="0"/>
+      <c r="HH3" s="0"/>
+      <c r="HI3" s="0"/>
+      <c r="HJ3" s="0"/>
+      <c r="HK3" s="0"/>
+      <c r="HL3" s="0"/>
+      <c r="HM3" s="0"/>
+      <c r="HN3" s="0"/>
+      <c r="HO3" s="0"/>
+      <c r="HP3" s="0"/>
+      <c r="HQ3" s="0"/>
+      <c r="HR3" s="0"/>
+      <c r="HS3" s="0"/>
+      <c r="HT3" s="0"/>
+      <c r="HU3" s="0"/>
+      <c r="HV3" s="0"/>
+      <c r="HW3" s="0"/>
+      <c r="HX3" s="0"/>
+      <c r="HY3" s="0"/>
+      <c r="HZ3" s="0"/>
+      <c r="IA3" s="0"/>
+      <c r="IB3" s="0"/>
+      <c r="IC3" s="0"/>
+      <c r="ID3" s="0"/>
+      <c r="IE3" s="0"/>
+      <c r="IF3" s="0"/>
+      <c r="IG3" s="0"/>
+      <c r="IH3" s="0"/>
+      <c r="II3" s="0"/>
+      <c r="IJ3" s="0"/>
+      <c r="IK3" s="0"/>
+      <c r="IL3" s="0"/>
+      <c r="IM3" s="0"/>
+      <c r="IN3" s="0"/>
+      <c r="IO3" s="0"/>
+      <c r="IP3" s="0"/>
+      <c r="IQ3" s="0"/>
+      <c r="IR3" s="0"/>
+      <c r="IS3" s="0"/>
+      <c r="IT3" s="0"/>
       <c r="IU3" s="0"/>
+      <c r="IV3" s="0"/>
+      <c r="IW3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A4" s="8" t="s">
@@ -515,10 +1012,258 @@
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="3"/>
+      <c r="F4" s="0"/>
       <c r="G4" s="7"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
+      <c r="J4" s="0"/>
+      <c r="K4" s="0"/>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0"/>
+      <c r="N4" s="0"/>
+      <c r="O4" s="0"/>
+      <c r="P4" s="0"/>
+      <c r="Q4" s="0"/>
+      <c r="R4" s="0"/>
+      <c r="S4" s="0"/>
+      <c r="T4" s="0"/>
+      <c r="U4" s="0"/>
+      <c r="V4" s="0"/>
+      <c r="W4" s="0"/>
+      <c r="X4" s="0"/>
+      <c r="Y4" s="0"/>
+      <c r="Z4" s="0"/>
+      <c r="AA4" s="0"/>
+      <c r="AB4" s="0"/>
+      <c r="AC4" s="0"/>
+      <c r="AD4" s="0"/>
+      <c r="AE4" s="0"/>
+      <c r="AF4" s="0"/>
+      <c r="AG4" s="0"/>
+      <c r="AH4" s="0"/>
+      <c r="AI4" s="0"/>
+      <c r="AJ4" s="0"/>
+      <c r="AK4" s="0"/>
+      <c r="AL4" s="0"/>
+      <c r="AM4" s="0"/>
+      <c r="AN4" s="0"/>
+      <c r="AO4" s="0"/>
+      <c r="AP4" s="0"/>
+      <c r="AQ4" s="0"/>
+      <c r="AR4" s="0"/>
+      <c r="AS4" s="0"/>
+      <c r="AT4" s="0"/>
+      <c r="AU4" s="0"/>
+      <c r="AV4" s="0"/>
+      <c r="AW4" s="0"/>
+      <c r="AX4" s="0"/>
+      <c r="AY4" s="0"/>
+      <c r="AZ4" s="0"/>
+      <c r="BA4" s="0"/>
+      <c r="BB4" s="0"/>
+      <c r="BC4" s="0"/>
+      <c r="BD4" s="0"/>
+      <c r="BE4" s="0"/>
+      <c r="BF4" s="0"/>
+      <c r="BG4" s="0"/>
+      <c r="BH4" s="0"/>
+      <c r="BI4" s="0"/>
+      <c r="BJ4" s="0"/>
+      <c r="BK4" s="0"/>
+      <c r="BL4" s="0"/>
+      <c r="BM4" s="0"/>
+      <c r="BN4" s="0"/>
+      <c r="BO4" s="0"/>
+      <c r="BP4" s="0"/>
+      <c r="BQ4" s="0"/>
+      <c r="BR4" s="0"/>
+      <c r="BS4" s="0"/>
+      <c r="BT4" s="0"/>
+      <c r="BU4" s="0"/>
+      <c r="BV4" s="0"/>
+      <c r="BW4" s="0"/>
+      <c r="BX4" s="0"/>
+      <c r="BY4" s="0"/>
+      <c r="BZ4" s="0"/>
+      <c r="CA4" s="0"/>
+      <c r="CB4" s="0"/>
+      <c r="CC4" s="0"/>
+      <c r="CD4" s="0"/>
+      <c r="CE4" s="0"/>
+      <c r="CF4" s="0"/>
+      <c r="CG4" s="0"/>
+      <c r="CH4" s="0"/>
+      <c r="CI4" s="0"/>
+      <c r="CJ4" s="0"/>
+      <c r="CK4" s="0"/>
+      <c r="CL4" s="0"/>
+      <c r="CM4" s="0"/>
+      <c r="CN4" s="0"/>
+      <c r="CO4" s="0"/>
+      <c r="CP4" s="0"/>
+      <c r="CQ4" s="0"/>
+      <c r="CR4" s="0"/>
+      <c r="CS4" s="0"/>
+      <c r="CT4" s="0"/>
+      <c r="CU4" s="0"/>
+      <c r="CV4" s="0"/>
+      <c r="CW4" s="0"/>
+      <c r="CX4" s="0"/>
+      <c r="CY4" s="0"/>
+      <c r="CZ4" s="0"/>
+      <c r="DA4" s="0"/>
+      <c r="DB4" s="0"/>
+      <c r="DC4" s="0"/>
+      <c r="DD4" s="0"/>
+      <c r="DE4" s="0"/>
+      <c r="DF4" s="0"/>
+      <c r="DG4" s="0"/>
+      <c r="DH4" s="0"/>
+      <c r="DI4" s="0"/>
+      <c r="DJ4" s="0"/>
+      <c r="DK4" s="0"/>
+      <c r="DL4" s="0"/>
+      <c r="DM4" s="0"/>
+      <c r="DN4" s="0"/>
+      <c r="DO4" s="0"/>
+      <c r="DP4" s="0"/>
+      <c r="DQ4" s="0"/>
+      <c r="DR4" s="0"/>
+      <c r="DS4" s="0"/>
+      <c r="DT4" s="0"/>
+      <c r="DU4" s="0"/>
+      <c r="DV4" s="0"/>
+      <c r="DW4" s="0"/>
+      <c r="DX4" s="0"/>
+      <c r="DY4" s="0"/>
+      <c r="DZ4" s="0"/>
+      <c r="EA4" s="0"/>
+      <c r="EB4" s="0"/>
+      <c r="EC4" s="0"/>
+      <c r="ED4" s="0"/>
+      <c r="EE4" s="0"/>
+      <c r="EF4" s="0"/>
+      <c r="EG4" s="0"/>
+      <c r="EH4" s="0"/>
+      <c r="EI4" s="0"/>
+      <c r="EJ4" s="0"/>
+      <c r="EK4" s="0"/>
+      <c r="EL4" s="0"/>
+      <c r="EM4" s="0"/>
+      <c r="EN4" s="0"/>
+      <c r="EO4" s="0"/>
+      <c r="EP4" s="0"/>
+      <c r="EQ4" s="0"/>
+      <c r="ER4" s="0"/>
+      <c r="ES4" s="0"/>
+      <c r="ET4" s="0"/>
+      <c r="EU4" s="0"/>
+      <c r="EV4" s="0"/>
+      <c r="EW4" s="0"/>
+      <c r="EX4" s="0"/>
+      <c r="EY4" s="0"/>
+      <c r="EZ4" s="0"/>
+      <c r="FA4" s="0"/>
+      <c r="FB4" s="0"/>
+      <c r="FC4" s="0"/>
+      <c r="FD4" s="0"/>
+      <c r="FE4" s="0"/>
+      <c r="FF4" s="0"/>
+      <c r="FG4" s="0"/>
+      <c r="FH4" s="0"/>
+      <c r="FI4" s="0"/>
+      <c r="FJ4" s="0"/>
+      <c r="FK4" s="0"/>
+      <c r="FL4" s="0"/>
+      <c r="FM4" s="0"/>
+      <c r="FN4" s="0"/>
+      <c r="FO4" s="0"/>
+      <c r="FP4" s="0"/>
+      <c r="FQ4" s="0"/>
+      <c r="FR4" s="0"/>
+      <c r="FS4" s="0"/>
+      <c r="FT4" s="0"/>
+      <c r="FU4" s="0"/>
+      <c r="FV4" s="0"/>
+      <c r="FW4" s="0"/>
+      <c r="FX4" s="0"/>
+      <c r="FY4" s="0"/>
+      <c r="FZ4" s="0"/>
+      <c r="GA4" s="0"/>
+      <c r="GB4" s="0"/>
+      <c r="GC4" s="0"/>
+      <c r="GD4" s="0"/>
+      <c r="GE4" s="0"/>
+      <c r="GF4" s="0"/>
+      <c r="GG4" s="0"/>
+      <c r="GH4" s="0"/>
+      <c r="GI4" s="0"/>
+      <c r="GJ4" s="0"/>
+      <c r="GK4" s="0"/>
+      <c r="GL4" s="0"/>
+      <c r="GM4" s="0"/>
+      <c r="GN4" s="0"/>
+      <c r="GO4" s="0"/>
+      <c r="GP4" s="0"/>
+      <c r="GQ4" s="0"/>
+      <c r="GR4" s="0"/>
+      <c r="GS4" s="0"/>
+      <c r="GT4" s="0"/>
+      <c r="GU4" s="0"/>
+      <c r="GV4" s="0"/>
+      <c r="GW4" s="0"/>
+      <c r="GX4" s="0"/>
+      <c r="GY4" s="0"/>
+      <c r="GZ4" s="0"/>
+      <c r="HA4" s="0"/>
+      <c r="HB4" s="0"/>
+      <c r="HC4" s="0"/>
+      <c r="HD4" s="0"/>
+      <c r="HE4" s="0"/>
+      <c r="HF4" s="0"/>
+      <c r="HG4" s="0"/>
+      <c r="HH4" s="0"/>
+      <c r="HI4" s="0"/>
+      <c r="HJ4" s="0"/>
+      <c r="HK4" s="0"/>
+      <c r="HL4" s="0"/>
+      <c r="HM4" s="0"/>
+      <c r="HN4" s="0"/>
+      <c r="HO4" s="0"/>
+      <c r="HP4" s="0"/>
+      <c r="HQ4" s="0"/>
+      <c r="HR4" s="0"/>
+      <c r="HS4" s="0"/>
+      <c r="HT4" s="0"/>
+      <c r="HU4" s="0"/>
+      <c r="HV4" s="0"/>
+      <c r="HW4" s="0"/>
+      <c r="HX4" s="0"/>
+      <c r="HY4" s="0"/>
+      <c r="HZ4" s="0"/>
+      <c r="IA4" s="0"/>
+      <c r="IB4" s="0"/>
+      <c r="IC4" s="0"/>
+      <c r="ID4" s="0"/>
+      <c r="IE4" s="0"/>
+      <c r="IF4" s="0"/>
+      <c r="IG4" s="0"/>
+      <c r="IH4" s="0"/>
+      <c r="II4" s="0"/>
+      <c r="IJ4" s="0"/>
+      <c r="IK4" s="0"/>
+      <c r="IL4" s="0"/>
+      <c r="IM4" s="0"/>
+      <c r="IN4" s="0"/>
+      <c r="IO4" s="0"/>
+      <c r="IP4" s="0"/>
+      <c r="IQ4" s="0"/>
+      <c r="IR4" s="0"/>
+      <c r="IS4" s="0"/>
+      <c r="IT4" s="0"/>
       <c r="IU4" s="0"/>
+      <c r="IV4" s="0"/>
+      <c r="IW4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="25.15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A5" s="8" t="s">
@@ -530,10 +1275,258 @@
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="3"/>
+      <c r="F5" s="0"/>
       <c r="G5" s="7"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
+      <c r="J5" s="0"/>
+      <c r="K5" s="0"/>
+      <c r="L5" s="0"/>
+      <c r="M5" s="0"/>
+      <c r="N5" s="0"/>
+      <c r="O5" s="0"/>
+      <c r="P5" s="0"/>
+      <c r="Q5" s="0"/>
+      <c r="R5" s="0"/>
+      <c r="S5" s="0"/>
+      <c r="T5" s="0"/>
+      <c r="U5" s="0"/>
+      <c r="V5" s="0"/>
+      <c r="W5" s="0"/>
+      <c r="X5" s="0"/>
+      <c r="Y5" s="0"/>
+      <c r="Z5" s="0"/>
+      <c r="AA5" s="0"/>
+      <c r="AB5" s="0"/>
+      <c r="AC5" s="0"/>
+      <c r="AD5" s="0"/>
+      <c r="AE5" s="0"/>
+      <c r="AF5" s="0"/>
+      <c r="AG5" s="0"/>
+      <c r="AH5" s="0"/>
+      <c r="AI5" s="0"/>
+      <c r="AJ5" s="0"/>
+      <c r="AK5" s="0"/>
+      <c r="AL5" s="0"/>
+      <c r="AM5" s="0"/>
+      <c r="AN5" s="0"/>
+      <c r="AO5" s="0"/>
+      <c r="AP5" s="0"/>
+      <c r="AQ5" s="0"/>
+      <c r="AR5" s="0"/>
+      <c r="AS5" s="0"/>
+      <c r="AT5" s="0"/>
+      <c r="AU5" s="0"/>
+      <c r="AV5" s="0"/>
+      <c r="AW5" s="0"/>
+      <c r="AX5" s="0"/>
+      <c r="AY5" s="0"/>
+      <c r="AZ5" s="0"/>
+      <c r="BA5" s="0"/>
+      <c r="BB5" s="0"/>
+      <c r="BC5" s="0"/>
+      <c r="BD5" s="0"/>
+      <c r="BE5" s="0"/>
+      <c r="BF5" s="0"/>
+      <c r="BG5" s="0"/>
+      <c r="BH5" s="0"/>
+      <c r="BI5" s="0"/>
+      <c r="BJ5" s="0"/>
+      <c r="BK5" s="0"/>
+      <c r="BL5" s="0"/>
+      <c r="BM5" s="0"/>
+      <c r="BN5" s="0"/>
+      <c r="BO5" s="0"/>
+      <c r="BP5" s="0"/>
+      <c r="BQ5" s="0"/>
+      <c r="BR5" s="0"/>
+      <c r="BS5" s="0"/>
+      <c r="BT5" s="0"/>
+      <c r="BU5" s="0"/>
+      <c r="BV5" s="0"/>
+      <c r="BW5" s="0"/>
+      <c r="BX5" s="0"/>
+      <c r="BY5" s="0"/>
+      <c r="BZ5" s="0"/>
+      <c r="CA5" s="0"/>
+      <c r="CB5" s="0"/>
+      <c r="CC5" s="0"/>
+      <c r="CD5" s="0"/>
+      <c r="CE5" s="0"/>
+      <c r="CF5" s="0"/>
+      <c r="CG5" s="0"/>
+      <c r="CH5" s="0"/>
+      <c r="CI5" s="0"/>
+      <c r="CJ5" s="0"/>
+      <c r="CK5" s="0"/>
+      <c r="CL5" s="0"/>
+      <c r="CM5" s="0"/>
+      <c r="CN5" s="0"/>
+      <c r="CO5" s="0"/>
+      <c r="CP5" s="0"/>
+      <c r="CQ5" s="0"/>
+      <c r="CR5" s="0"/>
+      <c r="CS5" s="0"/>
+      <c r="CT5" s="0"/>
+      <c r="CU5" s="0"/>
+      <c r="CV5" s="0"/>
+      <c r="CW5" s="0"/>
+      <c r="CX5" s="0"/>
+      <c r="CY5" s="0"/>
+      <c r="CZ5" s="0"/>
+      <c r="DA5" s="0"/>
+      <c r="DB5" s="0"/>
+      <c r="DC5" s="0"/>
+      <c r="DD5" s="0"/>
+      <c r="DE5" s="0"/>
+      <c r="DF5" s="0"/>
+      <c r="DG5" s="0"/>
+      <c r="DH5" s="0"/>
+      <c r="DI5" s="0"/>
+      <c r="DJ5" s="0"/>
+      <c r="DK5" s="0"/>
+      <c r="DL5" s="0"/>
+      <c r="DM5" s="0"/>
+      <c r="DN5" s="0"/>
+      <c r="DO5" s="0"/>
+      <c r="DP5" s="0"/>
+      <c r="DQ5" s="0"/>
+      <c r="DR5" s="0"/>
+      <c r="DS5" s="0"/>
+      <c r="DT5" s="0"/>
+      <c r="DU5" s="0"/>
+      <c r="DV5" s="0"/>
+      <c r="DW5" s="0"/>
+      <c r="DX5" s="0"/>
+      <c r="DY5" s="0"/>
+      <c r="DZ5" s="0"/>
+      <c r="EA5" s="0"/>
+      <c r="EB5" s="0"/>
+      <c r="EC5" s="0"/>
+      <c r="ED5" s="0"/>
+      <c r="EE5" s="0"/>
+      <c r="EF5" s="0"/>
+      <c r="EG5" s="0"/>
+      <c r="EH5" s="0"/>
+      <c r="EI5" s="0"/>
+      <c r="EJ5" s="0"/>
+      <c r="EK5" s="0"/>
+      <c r="EL5" s="0"/>
+      <c r="EM5" s="0"/>
+      <c r="EN5" s="0"/>
+      <c r="EO5" s="0"/>
+      <c r="EP5" s="0"/>
+      <c r="EQ5" s="0"/>
+      <c r="ER5" s="0"/>
+      <c r="ES5" s="0"/>
+      <c r="ET5" s="0"/>
+      <c r="EU5" s="0"/>
+      <c r="EV5" s="0"/>
+      <c r="EW5" s="0"/>
+      <c r="EX5" s="0"/>
+      <c r="EY5" s="0"/>
+      <c r="EZ5" s="0"/>
+      <c r="FA5" s="0"/>
+      <c r="FB5" s="0"/>
+      <c r="FC5" s="0"/>
+      <c r="FD5" s="0"/>
+      <c r="FE5" s="0"/>
+      <c r="FF5" s="0"/>
+      <c r="FG5" s="0"/>
+      <c r="FH5" s="0"/>
+      <c r="FI5" s="0"/>
+      <c r="FJ5" s="0"/>
+      <c r="FK5" s="0"/>
+      <c r="FL5" s="0"/>
+      <c r="FM5" s="0"/>
+      <c r="FN5" s="0"/>
+      <c r="FO5" s="0"/>
+      <c r="FP5" s="0"/>
+      <c r="FQ5" s="0"/>
+      <c r="FR5" s="0"/>
+      <c r="FS5" s="0"/>
+      <c r="FT5" s="0"/>
+      <c r="FU5" s="0"/>
+      <c r="FV5" s="0"/>
+      <c r="FW5" s="0"/>
+      <c r="FX5" s="0"/>
+      <c r="FY5" s="0"/>
+      <c r="FZ5" s="0"/>
+      <c r="GA5" s="0"/>
+      <c r="GB5" s="0"/>
+      <c r="GC5" s="0"/>
+      <c r="GD5" s="0"/>
+      <c r="GE5" s="0"/>
+      <c r="GF5" s="0"/>
+      <c r="GG5" s="0"/>
+      <c r="GH5" s="0"/>
+      <c r="GI5" s="0"/>
+      <c r="GJ5" s="0"/>
+      <c r="GK5" s="0"/>
+      <c r="GL5" s="0"/>
+      <c r="GM5" s="0"/>
+      <c r="GN5" s="0"/>
+      <c r="GO5" s="0"/>
+      <c r="GP5" s="0"/>
+      <c r="GQ5" s="0"/>
+      <c r="GR5" s="0"/>
+      <c r="GS5" s="0"/>
+      <c r="GT5" s="0"/>
+      <c r="GU5" s="0"/>
+      <c r="GV5" s="0"/>
+      <c r="GW5" s="0"/>
+      <c r="GX5" s="0"/>
+      <c r="GY5" s="0"/>
+      <c r="GZ5" s="0"/>
+      <c r="HA5" s="0"/>
+      <c r="HB5" s="0"/>
+      <c r="HC5" s="0"/>
+      <c r="HD5" s="0"/>
+      <c r="HE5" s="0"/>
+      <c r="HF5" s="0"/>
+      <c r="HG5" s="0"/>
+      <c r="HH5" s="0"/>
+      <c r="HI5" s="0"/>
+      <c r="HJ5" s="0"/>
+      <c r="HK5" s="0"/>
+      <c r="HL5" s="0"/>
+      <c r="HM5" s="0"/>
+      <c r="HN5" s="0"/>
+      <c r="HO5" s="0"/>
+      <c r="HP5" s="0"/>
+      <c r="HQ5" s="0"/>
+      <c r="HR5" s="0"/>
+      <c r="HS5" s="0"/>
+      <c r="HT5" s="0"/>
+      <c r="HU5" s="0"/>
+      <c r="HV5" s="0"/>
+      <c r="HW5" s="0"/>
+      <c r="HX5" s="0"/>
+      <c r="HY5" s="0"/>
+      <c r="HZ5" s="0"/>
+      <c r="IA5" s="0"/>
+      <c r="IB5" s="0"/>
+      <c r="IC5" s="0"/>
+      <c r="ID5" s="0"/>
+      <c r="IE5" s="0"/>
+      <c r="IF5" s="0"/>
+      <c r="IG5" s="0"/>
+      <c r="IH5" s="0"/>
+      <c r="II5" s="0"/>
+      <c r="IJ5" s="0"/>
+      <c r="IK5" s="0"/>
+      <c r="IL5" s="0"/>
+      <c r="IM5" s="0"/>
+      <c r="IN5" s="0"/>
+      <c r="IO5" s="0"/>
+      <c r="IP5" s="0"/>
+      <c r="IQ5" s="0"/>
+      <c r="IR5" s="0"/>
+      <c r="IS5" s="0"/>
+      <c r="IT5" s="0"/>
       <c r="IU5" s="0"/>
+      <c r="IV5" s="0"/>
+      <c r="IW5" s="0"/>
     </row>
     <row r="6" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="2"/>
@@ -548,11 +1541,259 @@
       <c r="D7" s="13"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
+      <c r="G7" s="0"/>
+      <c r="H7" s="0"/>
+      <c r="I7" s="0"/>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
+      <c r="L7" s="0"/>
+      <c r="M7" s="0"/>
+      <c r="N7" s="0"/>
+      <c r="O7" s="0"/>
+      <c r="P7" s="0"/>
+      <c r="Q7" s="0"/>
+      <c r="R7" s="0"/>
+      <c r="S7" s="0"/>
+      <c r="T7" s="0"/>
+      <c r="U7" s="0"/>
+      <c r="V7" s="0"/>
+      <c r="W7" s="0"/>
+      <c r="X7" s="0"/>
+      <c r="Y7" s="0"/>
+      <c r="Z7" s="0"/>
+      <c r="AA7" s="0"/>
+      <c r="AB7" s="0"/>
+      <c r="AC7" s="0"/>
+      <c r="AD7" s="0"/>
+      <c r="AE7" s="0"/>
+      <c r="AF7" s="0"/>
+      <c r="AG7" s="0"/>
+      <c r="AH7" s="0"/>
+      <c r="AI7" s="0"/>
+      <c r="AJ7" s="0"/>
+      <c r="AK7" s="0"/>
+      <c r="AL7" s="0"/>
+      <c r="AM7" s="0"/>
+      <c r="AN7" s="0"/>
+      <c r="AO7" s="0"/>
+      <c r="AP7" s="0"/>
+      <c r="AQ7" s="0"/>
+      <c r="AR7" s="0"/>
+      <c r="AS7" s="0"/>
+      <c r="AT7" s="0"/>
+      <c r="AU7" s="0"/>
+      <c r="AV7" s="0"/>
+      <c r="AW7" s="0"/>
+      <c r="AX7" s="0"/>
+      <c r="AY7" s="0"/>
+      <c r="AZ7" s="0"/>
+      <c r="BA7" s="0"/>
+      <c r="BB7" s="0"/>
+      <c r="BC7" s="0"/>
+      <c r="BD7" s="0"/>
+      <c r="BE7" s="0"/>
+      <c r="BF7" s="0"/>
+      <c r="BG7" s="0"/>
+      <c r="BH7" s="0"/>
+      <c r="BI7" s="0"/>
+      <c r="BJ7" s="0"/>
+      <c r="BK7" s="0"/>
+      <c r="BL7" s="0"/>
+      <c r="BM7" s="0"/>
+      <c r="BN7" s="0"/>
+      <c r="BO7" s="0"/>
+      <c r="BP7" s="0"/>
+      <c r="BQ7" s="0"/>
+      <c r="BR7" s="0"/>
+      <c r="BS7" s="0"/>
+      <c r="BT7" s="0"/>
+      <c r="BU7" s="0"/>
+      <c r="BV7" s="0"/>
+      <c r="BW7" s="0"/>
+      <c r="BX7" s="0"/>
+      <c r="BY7" s="0"/>
+      <c r="BZ7" s="0"/>
+      <c r="CA7" s="0"/>
+      <c r="CB7" s="0"/>
+      <c r="CC7" s="0"/>
+      <c r="CD7" s="0"/>
+      <c r="CE7" s="0"/>
+      <c r="CF7" s="0"/>
+      <c r="CG7" s="0"/>
+      <c r="CH7" s="0"/>
+      <c r="CI7" s="0"/>
+      <c r="CJ7" s="0"/>
+      <c r="CK7" s="0"/>
+      <c r="CL7" s="0"/>
+      <c r="CM7" s="0"/>
+      <c r="CN7" s="0"/>
+      <c r="CO7" s="0"/>
+      <c r="CP7" s="0"/>
+      <c r="CQ7" s="0"/>
+      <c r="CR7" s="0"/>
+      <c r="CS7" s="0"/>
+      <c r="CT7" s="0"/>
+      <c r="CU7" s="0"/>
+      <c r="CV7" s="0"/>
+      <c r="CW7" s="0"/>
+      <c r="CX7" s="0"/>
+      <c r="CY7" s="0"/>
+      <c r="CZ7" s="0"/>
+      <c r="DA7" s="0"/>
+      <c r="DB7" s="0"/>
+      <c r="DC7" s="0"/>
+      <c r="DD7" s="0"/>
+      <c r="DE7" s="0"/>
+      <c r="DF7" s="0"/>
+      <c r="DG7" s="0"/>
+      <c r="DH7" s="0"/>
+      <c r="DI7" s="0"/>
+      <c r="DJ7" s="0"/>
+      <c r="DK7" s="0"/>
+      <c r="DL7" s="0"/>
+      <c r="DM7" s="0"/>
+      <c r="DN7" s="0"/>
+      <c r="DO7" s="0"/>
+      <c r="DP7" s="0"/>
+      <c r="DQ7" s="0"/>
+      <c r="DR7" s="0"/>
+      <c r="DS7" s="0"/>
+      <c r="DT7" s="0"/>
+      <c r="DU7" s="0"/>
+      <c r="DV7" s="0"/>
+      <c r="DW7" s="0"/>
+      <c r="DX7" s="0"/>
+      <c r="DY7" s="0"/>
+      <c r="DZ7" s="0"/>
+      <c r="EA7" s="0"/>
+      <c r="EB7" s="0"/>
+      <c r="EC7" s="0"/>
+      <c r="ED7" s="0"/>
+      <c r="EE7" s="0"/>
+      <c r="EF7" s="0"/>
+      <c r="EG7" s="0"/>
+      <c r="EH7" s="0"/>
+      <c r="EI7" s="0"/>
+      <c r="EJ7" s="0"/>
+      <c r="EK7" s="0"/>
+      <c r="EL7" s="0"/>
+      <c r="EM7" s="0"/>
+      <c r="EN7" s="0"/>
+      <c r="EO7" s="0"/>
+      <c r="EP7" s="0"/>
+      <c r="EQ7" s="0"/>
+      <c r="ER7" s="0"/>
+      <c r="ES7" s="0"/>
+      <c r="ET7" s="0"/>
+      <c r="EU7" s="0"/>
+      <c r="EV7" s="0"/>
+      <c r="EW7" s="0"/>
+      <c r="EX7" s="0"/>
+      <c r="EY7" s="0"/>
+      <c r="EZ7" s="0"/>
+      <c r="FA7" s="0"/>
+      <c r="FB7" s="0"/>
+      <c r="FC7" s="0"/>
+      <c r="FD7" s="0"/>
+      <c r="FE7" s="0"/>
+      <c r="FF7" s="0"/>
+      <c r="FG7" s="0"/>
+      <c r="FH7" s="0"/>
+      <c r="FI7" s="0"/>
+      <c r="FJ7" s="0"/>
+      <c r="FK7" s="0"/>
+      <c r="FL7" s="0"/>
+      <c r="FM7" s="0"/>
+      <c r="FN7" s="0"/>
+      <c r="FO7" s="0"/>
+      <c r="FP7" s="0"/>
+      <c r="FQ7" s="0"/>
+      <c r="FR7" s="0"/>
+      <c r="FS7" s="0"/>
+      <c r="FT7" s="0"/>
+      <c r="FU7" s="0"/>
+      <c r="FV7" s="0"/>
+      <c r="FW7" s="0"/>
+      <c r="FX7" s="0"/>
+      <c r="FY7" s="0"/>
+      <c r="FZ7" s="0"/>
+      <c r="GA7" s="0"/>
+      <c r="GB7" s="0"/>
+      <c r="GC7" s="0"/>
+      <c r="GD7" s="0"/>
+      <c r="GE7" s="0"/>
+      <c r="GF7" s="0"/>
+      <c r="GG7" s="0"/>
+      <c r="GH7" s="0"/>
+      <c r="GI7" s="0"/>
+      <c r="GJ7" s="0"/>
+      <c r="GK7" s="0"/>
+      <c r="GL7" s="0"/>
+      <c r="GM7" s="0"/>
+      <c r="GN7" s="0"/>
+      <c r="GO7" s="0"/>
+      <c r="GP7" s="0"/>
+      <c r="GQ7" s="0"/>
+      <c r="GR7" s="0"/>
+      <c r="GS7" s="0"/>
+      <c r="GT7" s="0"/>
+      <c r="GU7" s="0"/>
+      <c r="GV7" s="0"/>
+      <c r="GW7" s="0"/>
+      <c r="GX7" s="0"/>
+      <c r="GY7" s="0"/>
+      <c r="GZ7" s="0"/>
+      <c r="HA7" s="0"/>
+      <c r="HB7" s="0"/>
+      <c r="HC7" s="0"/>
+      <c r="HD7" s="0"/>
+      <c r="HE7" s="0"/>
+      <c r="HF7" s="0"/>
+      <c r="HG7" s="0"/>
+      <c r="HH7" s="0"/>
+      <c r="HI7" s="0"/>
+      <c r="HJ7" s="0"/>
+      <c r="HK7" s="0"/>
+      <c r="HL7" s="0"/>
+      <c r="HM7" s="0"/>
+      <c r="HN7" s="0"/>
+      <c r="HO7" s="0"/>
+      <c r="HP7" s="0"/>
+      <c r="HQ7" s="0"/>
+      <c r="HR7" s="0"/>
+      <c r="HS7" s="0"/>
+      <c r="HT7" s="0"/>
+      <c r="HU7" s="0"/>
+      <c r="HV7" s="0"/>
+      <c r="HW7" s="0"/>
+      <c r="HX7" s="0"/>
+      <c r="HY7" s="0"/>
+      <c r="HZ7" s="0"/>
+      <c r="IA7" s="0"/>
+      <c r="IB7" s="0"/>
+      <c r="IC7" s="0"/>
+      <c r="ID7" s="0"/>
+      <c r="IE7" s="0"/>
+      <c r="IF7" s="0"/>
+      <c r="IG7" s="0"/>
+      <c r="IH7" s="0"/>
+      <c r="II7" s="0"/>
+      <c r="IJ7" s="0"/>
+      <c r="IK7" s="0"/>
+      <c r="IL7" s="0"/>
+      <c r="IM7" s="0"/>
+      <c r="IN7" s="0"/>
+      <c r="IO7" s="0"/>
+      <c r="IP7" s="0"/>
+      <c r="IQ7" s="0"/>
       <c r="IR7" s="0"/>
       <c r="IS7" s="0"/>
+      <c r="IT7" s="0"/>
       <c r="IU7" s="0"/>
+      <c r="IV7" s="0"/>
+      <c r="IW7" s="0"/>
     </row>
-    <row r="8" s="17" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="8" s="1" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A8" s="15" t="s">
         <v>8</v>
       </c>
@@ -564,7 +1805,7 @@
       </c>
       <c r="D8" s="0"/>
     </row>
-    <row r="9" s="17" customFormat="true" ht="14.65" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A9" s="15" t="s">
         <v>10</v>
       </c>
@@ -573,62 +1814,318 @@
         <v>11</v>
       </c>
       <c r="D9" s="0"/>
+      <c r="E9" s="0"/>
+      <c r="F9" s="0"/>
+      <c r="G9" s="0"/>
+      <c r="H9" s="0"/>
+      <c r="I9" s="0"/>
+      <c r="J9" s="0"/>
+      <c r="K9" s="0"/>
+      <c r="L9" s="0"/>
+      <c r="M9" s="0"/>
+      <c r="N9" s="0"/>
+      <c r="O9" s="0"/>
+      <c r="P9" s="0"/>
+      <c r="Q9" s="0"/>
+      <c r="R9" s="0"/>
+      <c r="S9" s="0"/>
+      <c r="T9" s="0"/>
+      <c r="U9" s="0"/>
+      <c r="V9" s="0"/>
+      <c r="W9" s="0"/>
+      <c r="X9" s="0"/>
+      <c r="Y9" s="0"/>
+      <c r="Z9" s="0"/>
+      <c r="AA9" s="0"/>
+      <c r="AB9" s="0"/>
+      <c r="AC9" s="0"/>
+      <c r="AD9" s="0"/>
+      <c r="AE9" s="0"/>
+      <c r="AF9" s="0"/>
+      <c r="AG9" s="0"/>
+      <c r="AH9" s="0"/>
+      <c r="AI9" s="0"/>
+      <c r="AJ9" s="0"/>
+      <c r="AK9" s="0"/>
+      <c r="AL9" s="0"/>
+      <c r="AM9" s="0"/>
+      <c r="AN9" s="0"/>
+      <c r="AO9" s="0"/>
+      <c r="AP9" s="0"/>
+      <c r="AQ9" s="0"/>
+      <c r="AR9" s="0"/>
+      <c r="AS9" s="0"/>
+      <c r="AT9" s="0"/>
+      <c r="AU9" s="0"/>
+      <c r="AV9" s="0"/>
+      <c r="AW9" s="0"/>
+      <c r="AX9" s="0"/>
+      <c r="AY9" s="0"/>
+      <c r="AZ9" s="0"/>
+      <c r="BA9" s="0"/>
+      <c r="BB9" s="0"/>
+      <c r="BC9" s="0"/>
+      <c r="BD9" s="0"/>
+      <c r="BE9" s="0"/>
+      <c r="BF9" s="0"/>
+      <c r="BG9" s="0"/>
+      <c r="BH9" s="0"/>
+      <c r="BI9" s="0"/>
+      <c r="BJ9" s="0"/>
+      <c r="BK9" s="0"/>
+      <c r="BL9" s="0"/>
+      <c r="BM9" s="0"/>
+      <c r="BN9" s="0"/>
+      <c r="BO9" s="0"/>
+      <c r="BP9" s="0"/>
+      <c r="BQ9" s="0"/>
+      <c r="BR9" s="0"/>
+      <c r="BS9" s="0"/>
+      <c r="BT9" s="0"/>
+      <c r="BU9" s="0"/>
+      <c r="BV9" s="0"/>
+      <c r="BW9" s="0"/>
+      <c r="BX9" s="0"/>
+      <c r="BY9" s="0"/>
+      <c r="BZ9" s="0"/>
+      <c r="CA9" s="0"/>
+      <c r="CB9" s="0"/>
+      <c r="CC9" s="0"/>
+      <c r="CD9" s="0"/>
+      <c r="CE9" s="0"/>
+      <c r="CF9" s="0"/>
+      <c r="CG9" s="0"/>
+      <c r="CH9" s="0"/>
+      <c r="CI9" s="0"/>
+      <c r="CJ9" s="0"/>
+      <c r="CK9" s="0"/>
+      <c r="CL9" s="0"/>
+      <c r="CM9" s="0"/>
+      <c r="CN9" s="0"/>
+      <c r="CO9" s="0"/>
+      <c r="CP9" s="0"/>
+      <c r="CQ9" s="0"/>
+      <c r="CR9" s="0"/>
+      <c r="CS9" s="0"/>
+      <c r="CT9" s="0"/>
+      <c r="CU9" s="0"/>
+      <c r="CV9" s="0"/>
+      <c r="CW9" s="0"/>
+      <c r="CX9" s="0"/>
+      <c r="CY9" s="0"/>
+      <c r="CZ9" s="0"/>
+      <c r="DA9" s="0"/>
+      <c r="DB9" s="0"/>
+      <c r="DC9" s="0"/>
+      <c r="DD9" s="0"/>
+      <c r="DE9" s="0"/>
+      <c r="DF9" s="0"/>
+      <c r="DG9" s="0"/>
+      <c r="DH9" s="0"/>
+      <c r="DI9" s="0"/>
+      <c r="DJ9" s="0"/>
+      <c r="DK9" s="0"/>
+      <c r="DL9" s="0"/>
+      <c r="DM9" s="0"/>
+      <c r="DN9" s="0"/>
+      <c r="DO9" s="0"/>
+      <c r="DP9" s="0"/>
+      <c r="DQ9" s="0"/>
+      <c r="DR9" s="0"/>
+      <c r="DS9" s="0"/>
+      <c r="DT9" s="0"/>
+      <c r="DU9" s="0"/>
+      <c r="DV9" s="0"/>
+      <c r="DW9" s="0"/>
+      <c r="DX9" s="0"/>
+      <c r="DY9" s="0"/>
+      <c r="DZ9" s="0"/>
+      <c r="EA9" s="0"/>
+      <c r="EB9" s="0"/>
+      <c r="EC9" s="0"/>
+      <c r="ED9" s="0"/>
+      <c r="EE9" s="0"/>
+      <c r="EF9" s="0"/>
+      <c r="EG9" s="0"/>
+      <c r="EH9" s="0"/>
+      <c r="EI9" s="0"/>
+      <c r="EJ9" s="0"/>
+      <c r="EK9" s="0"/>
+      <c r="EL9" s="0"/>
+      <c r="EM9" s="0"/>
+      <c r="EN9" s="0"/>
+      <c r="EO9" s="0"/>
+      <c r="EP9" s="0"/>
+      <c r="EQ9" s="0"/>
+      <c r="ER9" s="0"/>
+      <c r="ES9" s="0"/>
+      <c r="ET9" s="0"/>
+      <c r="EU9" s="0"/>
+      <c r="EV9" s="0"/>
+      <c r="EW9" s="0"/>
+      <c r="EX9" s="0"/>
+      <c r="EY9" s="0"/>
+      <c r="EZ9" s="0"/>
+      <c r="FA9" s="0"/>
+      <c r="FB9" s="0"/>
+      <c r="FC9" s="0"/>
+      <c r="FD9" s="0"/>
+      <c r="FE9" s="0"/>
+      <c r="FF9" s="0"/>
+      <c r="FG9" s="0"/>
+      <c r="FH9" s="0"/>
+      <c r="FI9" s="0"/>
+      <c r="FJ9" s="0"/>
+      <c r="FK9" s="0"/>
+      <c r="FL9" s="0"/>
+      <c r="FM9" s="0"/>
+      <c r="FN9" s="0"/>
+      <c r="FO9" s="0"/>
+      <c r="FP9" s="0"/>
+      <c r="FQ9" s="0"/>
+      <c r="FR9" s="0"/>
+      <c r="FS9" s="0"/>
+      <c r="FT9" s="0"/>
+      <c r="FU9" s="0"/>
+      <c r="FV9" s="0"/>
+      <c r="FW9" s="0"/>
+      <c r="FX9" s="0"/>
+      <c r="FY9" s="0"/>
+      <c r="FZ9" s="0"/>
+      <c r="GA9" s="0"/>
+      <c r="GB9" s="0"/>
+      <c r="GC9" s="0"/>
+      <c r="GD9" s="0"/>
+      <c r="GE9" s="0"/>
+      <c r="GF9" s="0"/>
+      <c r="GG9" s="0"/>
+      <c r="GH9" s="0"/>
+      <c r="GI9" s="0"/>
+      <c r="GJ9" s="0"/>
+      <c r="GK9" s="0"/>
+      <c r="GL9" s="0"/>
+      <c r="GM9" s="0"/>
+      <c r="GN9" s="0"/>
+      <c r="GO9" s="0"/>
+      <c r="GP9" s="0"/>
+      <c r="GQ9" s="0"/>
+      <c r="GR9" s="0"/>
+      <c r="GS9" s="0"/>
+      <c r="GT9" s="0"/>
+      <c r="GU9" s="0"/>
+      <c r="GV9" s="0"/>
+      <c r="GW9" s="0"/>
+      <c r="GX9" s="0"/>
+      <c r="GY9" s="0"/>
+      <c r="GZ9" s="0"/>
+      <c r="HA9" s="0"/>
+      <c r="HB9" s="0"/>
+      <c r="HC9" s="0"/>
+      <c r="HD9" s="0"/>
+      <c r="HE9" s="0"/>
+      <c r="HF9" s="0"/>
+      <c r="HG9" s="0"/>
+      <c r="HH9" s="0"/>
+      <c r="HI9" s="0"/>
+      <c r="HJ9" s="0"/>
+      <c r="HK9" s="0"/>
+      <c r="HL9" s="0"/>
+      <c r="HM9" s="0"/>
+      <c r="HN9" s="0"/>
+      <c r="HO9" s="0"/>
+      <c r="HP9" s="0"/>
+      <c r="HQ9" s="0"/>
+      <c r="HR9" s="0"/>
+      <c r="HS9" s="0"/>
+      <c r="HT9" s="0"/>
+      <c r="HU9" s="0"/>
+      <c r="HV9" s="0"/>
+      <c r="HW9" s="0"/>
+      <c r="HX9" s="0"/>
+      <c r="HY9" s="0"/>
+      <c r="HZ9" s="0"/>
+      <c r="IA9" s="0"/>
+      <c r="IB9" s="0"/>
+      <c r="IC9" s="0"/>
+      <c r="ID9" s="0"/>
+      <c r="IE9" s="0"/>
+      <c r="IF9" s="0"/>
+      <c r="IG9" s="0"/>
+      <c r="IH9" s="0"/>
+      <c r="II9" s="0"/>
+      <c r="IJ9" s="0"/>
+      <c r="IK9" s="0"/>
+      <c r="IL9" s="0"/>
+      <c r="IM9" s="0"/>
+      <c r="IN9" s="0"/>
+      <c r="IO9" s="0"/>
+      <c r="IP9" s="0"/>
+      <c r="IQ9" s="0"/>
+      <c r="IR9" s="0"/>
+      <c r="IS9" s="0"/>
+      <c r="IT9" s="0"/>
+      <c r="IU9" s="0"/>
+      <c r="IV9" s="0"/>
+      <c r="IW9" s="0"/>
     </row>
-    <row r="10" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A10" s="18" t="s">
+    <row r="10" s="19" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="0"/>
     </row>
     <row r="11" s="1" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="21" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="0"/>
       <c r="IR11" s="0"/>
       <c r="IS11" s="0"/>
     </row>
-    <row r="12" s="1" customFormat="true" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="23" t="s">
+    <row r="12" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="24" t="n">
+      <c r="B12" s="23" t="n">
         <v>21</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="23" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="0"/>
       <c r="IR12" s="0"/>
       <c r="IS12" s="0"/>
     </row>
-    <row r="13" s="1" customFormat="true" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="25" t="s">
+    <row r="13" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="24" t="n">
+      <c r="B13" s="23" t="n">
         <v>15</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="23" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="0"/>
       <c r="IR13" s="0"/>
       <c r="IS13" s="0"/>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="0"/>
+    </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>22</v>
@@ -645,7 +2142,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.15" right="0.140277777777778" top="0.179861111111111" bottom="0.2" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -660,18 +2157,18 @@
   </sheetPr>
   <dimension ref="A4:E7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="9.04"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -686,42 +2183,42 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="25" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="25" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="25" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>